<commit_message>
UN OCHA Briar updates
Briar's script run on these to remove legacy ArcGIS fields and the <Null> content in empty fields
</commit_message>
<xml_diff>
--- a/Data/GazetteerSqKm/GazetteerCombinedAdminLevels/ESH_AdminBoundaries_TabularData.xlsx
+++ b/Data/GazetteerSqKm/GazetteerCombinedAdminLevels/ESH_AdminBoundaries_TabularData.xlsx
@@ -15,22 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="41">
-  <si>
-    <t>OBJECTID_1</t>
-  </si>
-  <si>
-    <t>OBJECTID__</t>
-  </si>
-  <si>
-    <t>Shape__</t>
-  </si>
-  <si>
-    <t>Shape_Length</t>
-  </si>
-  <si>
-    <t>Shape_Area</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>admin0Name_en</t>
   </si>
@@ -65,15 +50,9 @@
     <t>validTo</t>
   </si>
   <si>
-    <t>OBJECTID</t>
-  </si>
-  <si>
     <t>Area_SqKm</t>
   </si>
   <si>
-    <t>Polygon</t>
-  </si>
-  <si>
     <t>Western Sahara</t>
   </si>
   <si>
@@ -81,9 +60,6 @@
   </si>
   <si>
     <t>EH</t>
-  </si>
-  <si>
-    <t>&lt;Null&gt;</t>
   </si>
   <si>
     <t>admin1Name_en</t>
@@ -499,13 +475,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -542,78 +531,24 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2">
-        <v>33.601516</v>
-      </c>
-      <c r="E2">
-        <v>23.857929</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="2">
+      <c r="I2" s="2">
         <v>42338</v>
       </c>
-      <c r="O2" s="2">
+      <c r="J2" s="2">
         <v>44291</v>
       </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2">
+      <c r="L2">
         <v>267319.8125</v>
       </c>
     </row>
@@ -624,289 +559,181 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2">
+        <v>42338</v>
+      </c>
+      <c r="J2" s="2">
+        <v>44291</v>
+      </c>
+      <c r="L2">
+        <v>43401.921875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="2">
+        <v>42338</v>
+      </c>
+      <c r="J3" s="2">
+        <v>44291</v>
+      </c>
+      <c r="L3">
+        <v>66943.421875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="2">
+        <v>42338</v>
+      </c>
+      <c r="J4" s="2">
+        <v>44291</v>
+      </c>
+      <c r="L4">
+        <v>30391.9453125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="B5" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="H5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2">
-        <v>10.638046</v>
-      </c>
-      <c r="E2">
-        <v>3.886799</v>
-      </c>
-      <c r="F2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="2">
+      <c r="I5" s="2">
         <v>42338</v>
       </c>
-      <c r="O2" s="2">
+      <c r="J5" s="2">
         <v>44291</v>
       </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>43401.921875</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3">
-        <v>10.55136</v>
-      </c>
-      <c r="E3">
-        <v>6.077189</v>
-      </c>
-      <c r="F3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" s="2">
-        <v>42338</v>
-      </c>
-      <c r="O3" s="2">
-        <v>44291</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3">
-        <v>2</v>
-      </c>
-      <c r="R3">
-        <v>66943.421875</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4">
-        <v>8.782147</v>
-      </c>
-      <c r="E4">
-        <v>2.754018</v>
-      </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="2">
-        <v>42338</v>
-      </c>
-      <c r="O4" s="2">
-        <v>44291</v>
-      </c>
-      <c r="P4" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q4">
-        <v>3</v>
-      </c>
-      <c r="R4">
-        <v>30391.9453125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5">
-        <v>20.32116</v>
-      </c>
-      <c r="E5">
-        <v>11.139922</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M5" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" s="2">
-        <v>42338</v>
-      </c>
-      <c r="O5" s="2">
-        <v>44291</v>
-      </c>
-      <c r="P5" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q5">
-        <v>4</v>
-      </c>
-      <c r="R5">
+      <c r="L5">
         <v>126582.5234375</v>
       </c>
     </row>

</xml_diff>